<commit_message>
20251103 8x Small/Smid caps
</commit_message>
<xml_diff>
--- a/GUI + Reviews/202509/DEZPT.xlsx
+++ b/GUI + Reviews/202509/DEZPT.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="V:\PM-Indices-IndexOperations\Review Files\202509\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://euronext-my.sharepoint.com/personal/csonneveld_euronext_com/Documents/Documents/Projects/GUI + Reviews/202509/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="0" documentId="8_{E51E7CD9-7B33-4911-8B2B-F73B44E673EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{2E4E4534-D795-44DF-BFF4-30B9EDC78CDF}"/>
+    <workbookView xWindow="-29115" yWindow="-16005" windowWidth="29040" windowHeight="15720" xr2:uid="{2E4E4534-D795-44DF-BFF4-30B9EDC78CDF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -4937,22 +4937,22 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4B95E4ED-5958-47B5-94A2-DF99FD9AE8B1}" name="Universe" displayName="Universe" ref="A1:M503" totalsRowShown="0" headerRowDxfId="1" dataDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4B95E4ED-5958-47B5-94A2-DF99FD9AE8B1}" name="Universe" displayName="Universe" ref="A1:M503" totalsRowShown="0" headerRowDxfId="14" dataDxfId="13">
   <autoFilter ref="A1:M503" xr:uid="{4B95E4ED-5958-47B5-94A2-DF99FD9AE8B1}"/>
   <tableColumns count="13">
-    <tableColumn id="1" xr3:uid="{FAA385F1-7C2A-4096-8083-08E64E492B2B}" name="Name" dataDxfId="14"/>
-    <tableColumn id="2" xr3:uid="{26C93A27-F400-4057-86D4-907FE6403208}" name="Ticker" dataDxfId="13"/>
-    <tableColumn id="3" xr3:uid="{7FA1F015-F697-42BF-A28E-0990A9113BDF}" name="ISIN" dataDxfId="12"/>
-    <tableColumn id="4" xr3:uid="{B30A343D-C1A0-454E-B697-F10ED6310F6F}" name="MIC" dataDxfId="11"/>
-    <tableColumn id="5" xr3:uid="{1166775A-6FE3-47C0-AB41-FB5D38CD8E4C}" name="Currency (Local)" dataDxfId="10"/>
-    <tableColumn id="6" xr3:uid="{9DBBE047-C57E-499D-80ED-EFDF8BE261F7}" name="Price (EUR) " dataDxfId="9"/>
-    <tableColumn id="7" xr3:uid="{58AC4C11-5D17-499E-A5C7-BF961F7A1BA0}" name="NOSH" dataDxfId="8"/>
-    <tableColumn id="8" xr3:uid="{9B70A8D0-B16C-4263-82B7-19764AC5611C}" name="20 days AVG turnover EUR" dataDxfId="7"/>
-    <tableColumn id="9" xr3:uid="{5DF6E9AF-9928-48FC-B221-D206D89DBC5C}" name="3M AVG Turnover EUR" dataDxfId="6"/>
-    <tableColumn id="10" xr3:uid="{47C7C2AE-F7F4-44E5-8F9A-BCC6727DF963}" name="3M AVG Turnover USD" dataDxfId="5"/>
-    <tableColumn id="11" xr3:uid="{1CA41BB9-E52C-4A9A-8F37-BDFBA38E1553}" name="100 Trading Days AVG Turnover EUR" dataDxfId="4"/>
-    <tableColumn id="12" xr3:uid="{B4FA96F2-BCEC-46EF-B028-28C98690E46B}" name="6M AVG Turnover EUR" dataDxfId="3"/>
-    <tableColumn id="13" xr3:uid="{C9AE0773-4B50-440D-A514-F43EAB6A3D78}" name="12M AVG Turnover EUR" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{FAA385F1-7C2A-4096-8083-08E64E492B2B}" name="Name" dataDxfId="12"/>
+    <tableColumn id="2" xr3:uid="{26C93A27-F400-4057-86D4-907FE6403208}" name="Ticker" dataDxfId="11"/>
+    <tableColumn id="3" xr3:uid="{7FA1F015-F697-42BF-A28E-0990A9113BDF}" name="ISIN" dataDxfId="10"/>
+    <tableColumn id="4" xr3:uid="{B30A343D-C1A0-454E-B697-F10ED6310F6F}" name="MIC" dataDxfId="9"/>
+    <tableColumn id="5" xr3:uid="{1166775A-6FE3-47C0-AB41-FB5D38CD8E4C}" name="Currency (Local)" dataDxfId="8"/>
+    <tableColumn id="6" xr3:uid="{9DBBE047-C57E-499D-80ED-EFDF8BE261F7}" name="Price (EUR) " dataDxfId="7"/>
+    <tableColumn id="7" xr3:uid="{58AC4C11-5D17-499E-A5C7-BF961F7A1BA0}" name="NOSH" dataDxfId="6"/>
+    <tableColumn id="8" xr3:uid="{9B70A8D0-B16C-4263-82B7-19764AC5611C}" name="20 days AVG turnover EUR" dataDxfId="5"/>
+    <tableColumn id="9" xr3:uid="{5DF6E9AF-9928-48FC-B221-D206D89DBC5C}" name="3M AVG Turnover EUR" dataDxfId="4"/>
+    <tableColumn id="10" xr3:uid="{47C7C2AE-F7F4-44E5-8F9A-BCC6727DF963}" name="3M AVG Turnover USD" dataDxfId="3"/>
+    <tableColumn id="11" xr3:uid="{1CA41BB9-E52C-4A9A-8F37-BDFBA38E1553}" name="100 Trading Days AVG Turnover EUR" dataDxfId="2"/>
+    <tableColumn id="12" xr3:uid="{B4FA96F2-BCEC-46EF-B028-28C98690E46B}" name="6M AVG Turnover EUR" dataDxfId="1"/>
+    <tableColumn id="13" xr3:uid="{C9AE0773-4B50-440D-A514-F43EAB6A3D78}" name="12M AVG Turnover EUR" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5277,7 +5277,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71D26D25-4C45-4AB8-B991-AD72F30E4673}">
   <dimension ref="A1:M503"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I14" sqref="I14"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>

</xml_diff>